<commit_message>
First Stable Version with UI (Limited Functions)
Two manufacturers available (only tested on few products)
Can't get dimensions from Rittal
</commit_message>
<xml_diff>
--- a/ProductIDs/rittal.xlsx
+++ b/ProductIDs/rittal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merno\Documents\GitHub\DataGrabber\ProductIDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A651C48F-16BD-48CE-ADB3-1EFB11E0B6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303BBCF5-5833-4E57-9540-561F7B004290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -367,6 +367,11 @@
         <v>1545000</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8001210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>